<commit_message>
Expand the test case.
</commit_message>
<xml_diff>
--- a/Data/Components.xlsx
+++ b/Data/Components.xlsx
@@ -47,7 +47,7 @@
     <t>Aap</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Expanded with Tsai Model.
</commit_message>
<xml_diff>
--- a/Data/Components.xlsx
+++ b/Data/Components.xlsx
@@ -411,7 +411,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +441,8 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <f>10^6</f>
+        <v>1000000</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -458,7 +459,8 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <f>10^6</f>
+        <v>1000000</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -475,7 +477,8 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <f>10^6</f>
+        <v>1000000</v>
       </c>
       <c r="D4">
         <v>1</v>

</xml_diff>